<commit_message>
Rw - Usage Update _1221PM
Boat Enabled
[2M] [10F Reserved] - [1F Mapped]

Boat Matrix - [-12]yd + [-1]td + (-3)ed
</commit_message>
<xml_diff>
--- a/System_2.1.6.xlsx
+++ b/System_2.1.6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CA2322-5527-4356-A987-5AEA45E3DDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5368EFF4-408B-4594-B394-3872E0EA3A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="623">
   <si>
     <t>Zone</t>
   </si>
@@ -1877,18 +1877,6 @@
     <t>Data in GB</t>
   </si>
   <si>
-    <t>Wbt_X_9F</t>
-  </si>
-  <si>
-    <t>12F Reserved</t>
-  </si>
-  <si>
-    <t>3M4F</t>
-  </si>
-  <si>
-    <t>6M</t>
-  </si>
-  <si>
     <t>X - Media - X</t>
   </si>
   <si>
@@ -1911,6 +1899,15 @@
   </si>
   <si>
     <t>X - Boat - X</t>
+  </si>
+  <si>
+    <t>Wbt_X_12F</t>
+  </si>
+  <si>
+    <t>2M11F</t>
+  </si>
+  <si>
+    <t>10F Reservered</t>
   </si>
 </sst>
 </file>
@@ -3497,7 +3494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="752">
+  <cellXfs count="748">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4820,6 +4817,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4868,6 +4875,72 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4898,62 +4971,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4979,12 +5157,6 @@
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -5006,161 +5178,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5219,18 +5247,6 @@
     <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5249,25 +5265,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5345,74 +5382,26 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5705,8 +5694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5762,10 +5751,10 @@
       <c r="I2" s="415" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="560" t="s">
+      <c r="J2" s="564" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="561"/>
+      <c r="K2" s="565"/>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5775,14 +5764,14 @@
       <c r="N2" s="361" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="562" t="s">
+      <c r="O2" s="566" t="s">
         <v>384</v>
       </c>
-      <c r="P2" s="563"/>
-      <c r="Q2" s="564"/>
-      <c r="R2" s="564"/>
-      <c r="S2" s="564"/>
-      <c r="T2" s="565" t="s">
+      <c r="P2" s="567"/>
+      <c r="Q2" s="568"/>
+      <c r="R2" s="568"/>
+      <c r="S2" s="568"/>
+      <c r="T2" s="569" t="s">
         <v>385</v>
       </c>
       <c r="V2" s="2" t="s">
@@ -5796,7 +5785,7 @@
       <c r="C3" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="557"/>
+      <c r="D3" s="561"/>
       <c r="E3" s="349"/>
       <c r="F3" s="271" t="s">
         <v>69</v>
@@ -5832,13 +5821,13 @@
       <c r="S3" s="24">
         <v>0</v>
       </c>
-      <c r="T3" s="566"/>
+      <c r="T3" s="570"/>
       <c r="U3" s="19" t="s">
         <v>587</v>
       </c>
       <c r="V3" s="19">
         <f>SUM(P3:P28)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5848,7 +5837,7 @@
       <c r="C4" s="168" t="s">
         <v>361</v>
       </c>
-      <c r="D4" s="558"/>
+      <c r="D4" s="562"/>
       <c r="E4" s="61"/>
       <c r="F4" s="371" t="s">
         <v>42</v>
@@ -5865,7 +5854,7 @@
       </c>
       <c r="O4" s="6"/>
       <c r="P4" s="321"/>
-      <c r="T4" s="566"/>
+      <c r="T4" s="570"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -5874,7 +5863,7 @@
       <c r="C5" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="559"/>
+      <c r="D5" s="563"/>
       <c r="F5" s="375" t="s">
         <v>42</v>
       </c>
@@ -5893,7 +5882,7 @@
         <v>521</v>
       </c>
       <c r="P5" s="321"/>
-      <c r="T5" s="566"/>
+      <c r="T5" s="570"/>
       <c r="U5" s="209" t="s">
         <v>228</v>
       </c>
@@ -5932,7 +5921,7 @@
       <c r="P6" s="321"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="6"/>
-      <c r="T6" s="566"/>
+      <c r="T6" s="570"/>
     </row>
     <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="214" t="s">
@@ -5972,7 +5961,7 @@
       <c r="S7" s="24">
         <v>1</v>
       </c>
-      <c r="T7" s="566"/>
+      <c r="T7" s="570"/>
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -6001,7 +5990,7 @@
       <c r="P8" s="321"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="6"/>
-      <c r="T8" s="566"/>
+      <c r="T8" s="570"/>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -6034,8 +6023,16 @@
       <c r="O9" s="500" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="321"/>
-      <c r="T9" s="566"/>
+      <c r="P9" s="321">
+        <v>1</v>
+      </c>
+      <c r="R9" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="S9" s="24">
+        <v>1</v>
+      </c>
+      <c r="T9" s="570"/>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -6065,7 +6062,7 @@
         <v>521</v>
       </c>
       <c r="P10" s="321"/>
-      <c r="T10" s="566"/>
+      <c r="T10" s="570"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -6107,7 +6104,7 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="T11" s="566"/>
+      <c r="T11" s="570"/>
       <c r="U11" s="209" t="s">
         <v>227</v>
       </c>
@@ -6140,7 +6137,7 @@
       <c r="P12" s="321"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="142"/>
-      <c r="T12" s="566"/>
+      <c r="T12" s="570"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="261" t="s">
@@ -6172,7 +6169,7 @@
       </c>
       <c r="P13" s="321"/>
       <c r="R13" s="142"/>
-      <c r="T13" s="566"/>
+      <c r="T13" s="570"/>
       <c r="U13" s="2" t="s">
         <v>611</v>
       </c>
@@ -6182,7 +6179,7 @@
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P14" s="321"/>
-      <c r="T14" s="566"/>
+      <c r="T14" s="570"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -6208,10 +6205,10 @@
       <c r="L15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="554">
+      <c r="M15" s="558">
         <v>45275</v>
       </c>
-      <c r="N15" s="557" t="s">
+      <c r="N15" s="561" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="500" t="s">
@@ -6229,7 +6226,7 @@
       <c r="S15" s="24">
         <v>1</v>
       </c>
-      <c r="T15" s="566"/>
+      <c r="T15" s="570"/>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="486" t="s">
@@ -6255,9 +6252,11 @@
       <c r="L16" s="199" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="555"/>
-      <c r="N16" s="558"/>
-      <c r="P16" s="321"/>
+      <c r="M16" s="559"/>
+      <c r="N16" s="562"/>
+      <c r="P16" s="321">
+        <v>1</v>
+      </c>
       <c r="Q16" s="19" t="s">
         <v>607</v>
       </c>
@@ -6267,7 +6266,7 @@
       <c r="S16" s="112">
         <v>1</v>
       </c>
-      <c r="T16" s="566"/>
+      <c r="T16" s="570"/>
     </row>
     <row r="17" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -6295,8 +6294,8 @@
       <c r="L17" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="556"/>
-      <c r="N17" s="559"/>
+      <c r="M17" s="560"/>
+      <c r="N17" s="563"/>
       <c r="O17" s="500" t="s">
         <v>44</v>
       </c>
@@ -6312,11 +6311,11 @@
       <c r="S17" s="24">
         <v>0</v>
       </c>
-      <c r="T17" s="566"/>
+      <c r="T17" s="570"/>
     </row>
     <row r="18" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="321"/>
-      <c r="T18" s="566"/>
+      <c r="T18" s="570"/>
     </row>
     <row r="19" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -6344,14 +6343,14 @@
       <c r="L19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="554">
+      <c r="M19" s="558">
         <v>45275</v>
       </c>
       <c r="N19" s="414" t="s">
         <v>521</v>
       </c>
       <c r="P19" s="321"/>
-      <c r="T19" s="566"/>
+      <c r="T19" s="570"/>
     </row>
     <row r="20" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="246" t="s">
@@ -6377,7 +6376,7 @@
       <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="555"/>
+      <c r="M20" s="559"/>
       <c r="N20" s="404" t="s">
         <v>26</v>
       </c>
@@ -6393,7 +6392,7 @@
       <c r="S20" s="24">
         <v>1</v>
       </c>
-      <c r="T20" s="566"/>
+      <c r="T20" s="570"/>
     </row>
     <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="246" t="s">
@@ -6419,11 +6418,13 @@
       <c r="L21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="555"/>
+      <c r="M21" s="559"/>
       <c r="N21" s="404" t="s">
         <v>18</v>
       </c>
-      <c r="P21" s="321"/>
+      <c r="P21" s="321">
+        <v>1</v>
+      </c>
       <c r="Q21" s="19" t="s">
         <v>208</v>
       </c>
@@ -6433,11 +6434,11 @@
       <c r="S21" s="24">
         <v>1</v>
       </c>
-      <c r="T21" s="566"/>
-      <c r="U21" s="552" t="s">
+      <c r="T21" s="570"/>
+      <c r="U21" s="556" t="s">
         <v>226</v>
       </c>
-      <c r="V21" s="553"/>
+      <c r="V21" s="557"/>
     </row>
     <row r="22" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="276" t="s">
@@ -6463,14 +6464,14 @@
       <c r="L22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="555"/>
+      <c r="M22" s="559"/>
       <c r="N22" s="384" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="321"/>
-      <c r="T22" s="566"/>
+      <c r="T22" s="570"/>
       <c r="X22" s="19" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
     </row>
     <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6497,14 +6498,14 @@
       <c r="L23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="555"/>
+      <c r="M23" s="559"/>
       <c r="N23" s="61" t="s">
         <v>522</v>
       </c>
       <c r="P23" s="321"/>
-      <c r="T23" s="566"/>
+      <c r="T23" s="570"/>
       <c r="U23" s="2" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="V23" s="100" t="s">
         <v>44</v>
@@ -6537,7 +6538,7 @@
       <c r="L24" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="555"/>
+      <c r="M24" s="559"/>
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
@@ -6546,7 +6547,7 @@
       </c>
       <c r="P24" s="549"/>
       <c r="S24" s="80"/>
-      <c r="T24" s="566"/>
+      <c r="T24" s="570"/>
     </row>
     <row r="25" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
@@ -6574,7 +6575,7 @@
       <c r="L25" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="555"/>
+      <c r="M25" s="559"/>
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
@@ -6590,10 +6591,8 @@
       <c r="S25" s="21">
         <v>0</v>
       </c>
-      <c r="T25" s="566"/>
-      <c r="V25" s="19" t="s">
-        <v>615</v>
-      </c>
+      <c r="T25" s="570"/>
+      <c r="V25" s="19"/>
     </row>
     <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
@@ -6619,14 +6618,14 @@
       <c r="L26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="555"/>
+      <c r="M26" s="559"/>
       <c r="N26" s="61" t="s">
         <v>523</v>
       </c>
       <c r="P26" s="321"/>
-      <c r="T26" s="566"/>
+      <c r="T26" s="570"/>
       <c r="V26" s="550" t="s">
-        <v>614</v>
+        <v>621</v>
       </c>
     </row>
     <row r="27" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6649,7 +6648,7 @@
       <c r="J27" s="411"/>
       <c r="K27" s="412"/>
       <c r="L27" s="413"/>
-      <c r="M27" s="555"/>
+      <c r="M27" s="559"/>
       <c r="N27" s="61"/>
       <c r="P27" s="321">
         <v>1</v>
@@ -6663,7 +6662,7 @@
       <c r="S27" s="24">
         <v>0</v>
       </c>
-      <c r="T27" s="566"/>
+      <c r="T27" s="570"/>
       <c r="W27" s="2" t="s">
         <v>603</v>
       </c>
@@ -6692,7 +6691,7 @@
       <c r="L28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="556"/>
+      <c r="M28" s="560"/>
       <c r="N28" s="61" t="s">
         <v>523</v>
       </c>
@@ -6708,7 +6707,7 @@
       <c r="S28" s="21">
         <v>0</v>
       </c>
-      <c r="T28" s="567"/>
+      <c r="T28" s="571"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6730,7 +6729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AH19" sqref="AH19"/>
     </sheetView>
   </sheetViews>
@@ -6798,7 +6797,7 @@
       <c r="P1" s="422" t="s">
         <v>407</v>
       </c>
-      <c r="Q1" s="571" t="s">
+      <c r="Q1" s="597" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6819,14 +6818,14 @@
       <c r="Z1" s="24" t="s">
         <v>587</v>
       </c>
-      <c r="AA1" s="748" t="s">
+      <c r="AA1" s="555" t="s">
         <v>454</v>
       </c>
-      <c r="AB1" s="749" t="s">
-        <v>622</v>
+      <c r="AB1" s="572" t="s">
+        <v>618</v>
       </c>
       <c r="AC1" s="99" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="AD1" s="355"/>
       <c r="AE1" s="19" t="s">
@@ -6839,35 +6838,35 @@
       <c r="AH1" s="355"/>
       <c r="AI1" s="355"/>
       <c r="AJ1" s="355"/>
-      <c r="AK1" s="741"/>
+      <c r="AK1" s="552"/>
     </row>
     <row r="2" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="581">
+      <c r="A2" s="578">
         <f ca="1">TODAY()</f>
-        <v>45280</v>
-      </c>
-      <c r="B2" s="583" t="s">
+        <v>45281</v>
+      </c>
+      <c r="B2" s="580" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="595" t="s">
+      <c r="C2" s="592" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="585" t="s">
+      <c r="D2" s="582" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="587" t="s">
+      <c r="E2" s="584" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="593" t="s">
+      <c r="G2" s="590" t="s">
         <v>380</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="575" t="s">
+      <c r="I2" s="601" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="420" t="s">
@@ -6891,7 +6890,7 @@
       <c r="P2" s="423">
         <v>40</v>
       </c>
-      <c r="Q2" s="572"/>
+      <c r="Q2" s="598"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>4</v>
@@ -6914,32 +6913,28 @@
       <c r="X2" s="495"/>
       <c r="Z2" s="24">
         <f>BoardRW!V3</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AA2" s="68">
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="750"/>
+      <c r="AB2" s="573"/>
       <c r="AC2" s="35"/>
-      <c r="AD2" s="742"/>
-      <c r="AE2" s="742"/>
-      <c r="AF2" s="742"/>
-      <c r="AG2" s="742"/>
-      <c r="AH2" s="743"/>
+      <c r="AH2" s="6"/>
       <c r="AI2" s="495"/>
-      <c r="AJ2" s="743"/>
+      <c r="AJ2" s="6"/>
       <c r="AK2" s="495"/>
     </row>
     <row r="3" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="582"/>
-      <c r="B3" s="584"/>
-      <c r="C3" s="596"/>
-      <c r="D3" s="586"/>
-      <c r="E3" s="588"/>
-      <c r="G3" s="594"/>
+      <c r="A3" s="579"/>
+      <c r="B3" s="581"/>
+      <c r="C3" s="593"/>
+      <c r="D3" s="583"/>
+      <c r="E3" s="585"/>
+      <c r="G3" s="591"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="576"/>
+      <c r="I3" s="602"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6958,20 +6953,19 @@
         <v>252</v>
       </c>
       <c r="X3" s="496"/>
-      <c r="AB3" s="750"/>
+      <c r="AB3" s="573"/>
       <c r="AC3" s="35"/>
-      <c r="AD3" s="742"/>
       <c r="AE3" s="100" t="s">
-        <v>617</v>
-      </c>
-      <c r="AF3" s="744"/>
+        <v>613</v>
+      </c>
+      <c r="AF3" s="20"/>
       <c r="AG3" s="24">
         <f>IF((AE7-SUM(AI2:AI10)&lt;0),AE7-SUM(AK2:AK10),0)</f>
         <v>0</v>
       </c>
-      <c r="AH3" s="743"/>
+      <c r="AH3" s="6"/>
       <c r="AI3" s="496"/>
-      <c r="AJ3" s="743"/>
+      <c r="AJ3" s="6"/>
       <c r="AK3" s="496"/>
     </row>
     <row r="4" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6979,12 +6973,12 @@
         <v>389</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="589" t="s">
+      <c r="C4" s="586" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="576"/>
+      <c r="I4" s="602"/>
       <c r="R4" s="497" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="T4" s="24">
         <f>IF((R7-SUM(X2:X10)&lt;0),R7-SUM(V2:V10),0)</f>
@@ -7000,20 +6994,19 @@
       <c r="X4" s="496">
         <v>1</v>
       </c>
-      <c r="AB4" s="750"/>
+      <c r="AB4" s="573"/>
       <c r="AC4" s="35"/>
-      <c r="AD4" s="742"/>
-      <c r="AE4" s="744"/>
+      <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="AG4" s="24">
         <f>IF((AE8-SUM(AK2:AK10)&lt;0),AE8-SUM(AK2:AK10),0)</f>
         <v>0</v>
       </c>
-      <c r="AH4" s="743"/>
+      <c r="AH4" s="6"/>
       <c r="AI4" s="496"/>
-      <c r="AJ4" s="743"/>
+      <c r="AJ4" s="6"/>
       <c r="AK4" s="496"/>
     </row>
     <row r="5" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7023,7 +7016,7 @@
       <c r="B5" s="100" t="s">
         <v>364</v>
       </c>
-      <c r="C5" s="590"/>
+      <c r="C5" s="587"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -7033,13 +7026,13 @@
       <c r="F5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="557" t="s">
+      <c r="G5" s="561" t="s">
         <v>276</v>
       </c>
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="576"/>
+      <c r="I5" s="602"/>
       <c r="J5" s="421" t="s">
         <v>273</v>
       </c>
@@ -7056,7 +7049,7 @@
         <v>317</v>
       </c>
       <c r="S5" s="497" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="T5" s="24">
         <f>IF((S7-SUM(V2:V10))&lt;0,S7-SUM(X2:X10),0)</f>
@@ -7068,35 +7061,31 @@
       <c r="V5" s="494"/>
       <c r="W5" s="6"/>
       <c r="X5" s="494"/>
-      <c r="AB5" s="750"/>
+      <c r="AB5" s="573"/>
       <c r="AC5" s="35"/>
-      <c r="AD5" s="742"/>
-      <c r="AE5" s="742"/>
-      <c r="AF5" s="742"/>
-      <c r="AG5" s="742"/>
-      <c r="AH5" s="743"/>
+      <c r="AH5" s="6"/>
       <c r="AI5" s="494">
         <v>0</v>
       </c>
-      <c r="AJ5" s="743"/>
+      <c r="AJ5" s="6"/>
       <c r="AK5" s="494"/>
     </row>
     <row r="6" spans="1:37" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="578" t="s">
+      <c r="A6" s="575" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="591"/>
-      <c r="D6" s="592"/>
+      <c r="C6" s="588"/>
+      <c r="D6" s="589"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
-      <c r="G6" s="558"/>
-      <c r="I6" s="576"/>
+      <c r="G6" s="562"/>
+      <c r="I6" s="602"/>
       <c r="P6" s="61" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="R6" s="64">
         <f>R7-SUM(X2:X10)+R11</f>
@@ -7106,19 +7095,13 @@
         <f>S7-S12-SUM(V2:V10)</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="750"/>
+      <c r="AB6" s="573"/>
       <c r="AC6" s="35"/>
-      <c r="AD6" s="742"/>
-      <c r="AE6" s="742"/>
-      <c r="AF6" s="742"/>
-      <c r="AG6" s="742"/>
-      <c r="AH6" s="742"/>
-      <c r="AI6" s="744"/>
-      <c r="AJ6" s="742"/>
+      <c r="AI6" s="20"/>
       <c r="AK6" s="342"/>
     </row>
     <row r="7" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="579"/>
+      <c r="A7" s="576"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -7128,8 +7111,8 @@
       <c r="D7" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="558"/>
-      <c r="I7" s="576"/>
+      <c r="G7" s="562"/>
+      <c r="I7" s="602"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -7165,9 +7148,9 @@
       <c r="X7" s="495">
         <v>1</v>
       </c>
-      <c r="AB7" s="750"/>
+      <c r="AB7" s="573"/>
       <c r="AC7" s="99" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="AD7" s="127" t="s">
         <v>44</v>
@@ -7180,16 +7163,15 @@
         <f>3-AF11-SUM(AK1:AK10)</f>
         <v>0</v>
       </c>
-      <c r="AG7" s="742"/>
-      <c r="AH7" s="743"/>
+      <c r="AH7" s="6"/>
       <c r="AI7" s="495">
         <v>0</v>
       </c>
-      <c r="AJ7" s="743"/>
+      <c r="AJ7" s="6"/>
       <c r="AK7" s="495"/>
     </row>
     <row r="8" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="580"/>
+      <c r="A8" s="577"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -7197,8 +7179,8 @@
       <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="558"/>
-      <c r="I8" s="576"/>
+      <c r="G8" s="562"/>
+      <c r="I8" s="602"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>465</v>
@@ -7208,17 +7190,15 @@
       </c>
       <c r="W8" s="6"/>
       <c r="X8" s="492"/>
-      <c r="AB8" s="750"/>
-      <c r="AC8" s="745"/>
-      <c r="AD8" s="742"/>
-      <c r="AE8" s="744"/>
-      <c r="AF8" s="744"/>
-      <c r="AG8" s="742"/>
-      <c r="AH8" s="743"/>
+      <c r="AB8" s="573"/>
+      <c r="AC8" s="553"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
+      <c r="AH8" s="6"/>
       <c r="AI8" s="24">
         <v>0</v>
       </c>
-      <c r="AJ8" s="743"/>
+      <c r="AJ8" s="6"/>
       <c r="AK8" s="492"/>
     </row>
     <row r="9" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7234,9 +7214,9 @@
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="558"/>
+      <c r="G9" s="562"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="576"/>
+      <c r="I9" s="602"/>
       <c r="M9" s="19" t="s">
         <v>545</v>
       </c>
@@ -7246,15 +7226,12 @@
       </c>
       <c r="V9" s="24"/>
       <c r="X9" s="492"/>
-      <c r="AB9" s="750"/>
-      <c r="AC9" s="745"/>
-      <c r="AD9" s="742"/>
-      <c r="AE9" s="744"/>
-      <c r="AF9" s="744"/>
-      <c r="AG9" s="742"/>
-      <c r="AH9" s="743"/>
+      <c r="AB9" s="573"/>
+      <c r="AC9" s="553"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AH9" s="6"/>
       <c r="AI9" s="24"/>
-      <c r="AJ9" s="742"/>
       <c r="AK9" s="492"/>
     </row>
     <row r="10" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7270,8 +7247,8 @@
         <f>Boat!U8</f>
         <v>37</v>
       </c>
-      <c r="G10" s="558"/>
-      <c r="I10" s="576"/>
+      <c r="G10" s="562"/>
+      <c r="I10" s="602"/>
       <c r="J10" s="24" t="s">
         <v>380</v>
       </c>
@@ -7288,22 +7265,20 @@
       <c r="V10" s="496"/>
       <c r="W10" s="6"/>
       <c r="X10" s="492"/>
-      <c r="AB10" s="750"/>
-      <c r="AC10" s="745"/>
-      <c r="AD10" s="742"/>
-      <c r="AE10" s="744"/>
-      <c r="AF10" s="744"/>
-      <c r="AG10" s="742"/>
-      <c r="AH10" s="743"/>
+      <c r="AB10" s="573"/>
+      <c r="AC10" s="553"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AH10" s="6"/>
       <c r="AI10" s="496"/>
-      <c r="AJ10" s="743"/>
+      <c r="AJ10" s="6"/>
       <c r="AK10" s="492"/>
     </row>
     <row r="11" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="557" t="s">
+      <c r="B11" s="561" t="s">
         <v>391</v>
       </c>
       <c r="C11" s="175" t="s">
@@ -7312,8 +7287,8 @@
       <c r="D11" s="222" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="558"/>
-      <c r="I11" s="576"/>
+      <c r="G11" s="562"/>
+      <c r="I11" s="602"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7339,15 +7314,15 @@
       <c r="S11" s="24">
         <v>0</v>
       </c>
-      <c r="U11" s="568" t="s">
+      <c r="U11" s="594" t="s">
         <v>579</v>
       </c>
-      <c r="V11" s="569"/>
-      <c r="W11" s="569"/>
-      <c r="X11" s="570"/>
-      <c r="AB11" s="751"/>
+      <c r="V11" s="595"/>
+      <c r="W11" s="595"/>
+      <c r="X11" s="596"/>
+      <c r="AB11" s="574"/>
       <c r="AC11" s="99" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="AD11" s="127" t="s">
         <v>44</v>
@@ -7359,23 +7334,23 @@
         <v>3</v>
       </c>
       <c r="AG11" s="438"/>
-      <c r="AH11" s="568" t="s">
+      <c r="AH11" s="594" t="s">
         <v>579</v>
       </c>
-      <c r="AI11" s="569"/>
-      <c r="AJ11" s="569"/>
-      <c r="AK11" s="570"/>
+      <c r="AI11" s="595"/>
+      <c r="AJ11" s="595"/>
+      <c r="AK11" s="596"/>
     </row>
     <row r="12" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
         <v>392</v>
       </c>
-      <c r="B12" s="559"/>
+      <c r="B12" s="563"/>
       <c r="E12" s="234">
         <v>3</v>
       </c>
-      <c r="G12" s="558"/>
-      <c r="I12" s="576"/>
+      <c r="G12" s="562"/>
+      <c r="I12" s="602"/>
       <c r="J12" s="24" t="s">
         <v>536</v>
       </c>
@@ -7403,12 +7378,12 @@
       <c r="B13" s="221" t="s">
         <v>330</v>
       </c>
-      <c r="C13" s="557" t="s">
+      <c r="C13" s="561" t="s">
         <v>195</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="G13" s="558"/>
-      <c r="I13" s="576"/>
+      <c r="G13" s="562"/>
+      <c r="I13" s="602"/>
       <c r="J13" s="108" t="s">
         <v>569</v>
       </c>
@@ -7427,7 +7402,7 @@
       <c r="U13" s="6"/>
       <c r="V13" s="112"/>
       <c r="W13" s="6"/>
-      <c r="Z13" s="746" t="s">
+      <c r="Z13" s="554" t="s">
         <v>260</v>
       </c>
     </row>
@@ -7438,7 +7413,7 @@
       <c r="B14" s="177" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="559"/>
+      <c r="C14" s="563"/>
       <c r="D14" s="209" t="s">
         <v>154</v>
       </c>
@@ -7448,11 +7423,11 @@
       <c r="F14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="G14" s="559"/>
+      <c r="G14" s="563"/>
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="576"/>
+      <c r="I14" s="602"/>
       <c r="U14" s="67" t="s">
         <v>81</v>
       </c>
@@ -7479,7 +7454,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="576"/>
+      <c r="I15" s="602"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7493,7 +7468,7 @@
         <v>416</v>
       </c>
       <c r="R15" s="497" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="T15" s="24">
         <f>IF((R18-SUM(X16:X21))&lt;0,R18-SUM(X16:X21),0)</f>
@@ -7510,13 +7485,13 @@
       <c r="D16" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="I16" s="576"/>
+      <c r="I16" s="602"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
       <c r="L16" s="6"/>
       <c r="S16" s="497" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="T16" s="21">
         <f>IF((S18-SUM(V16:V21))&lt;0,S18-SUM(V16:V21),0)</f>
@@ -7554,7 +7529,7 @@
       <c r="G17" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I17" s="576"/>
+      <c r="I17" s="602"/>
       <c r="L17" s="2" t="s">
         <v>443</v>
       </c>
@@ -7572,17 +7547,17 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="576"/>
+      <c r="I18" s="602"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="573" t="s">
+      <c r="O18" s="599" t="s">
         <v>537</v>
       </c>
-      <c r="P18" s="574"/>
+      <c r="P18" s="600"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="R18" s="747">
+      <c r="R18" s="24">
         <f>5-R26</f>
         <v>3</v>
       </c>
@@ -7604,7 +7579,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="576"/>
+      <c r="I19" s="602"/>
       <c r="M19" s="21" t="s">
         <v>442</v>
       </c>
@@ -7640,7 +7615,7 @@
       <c r="G20" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I20" s="576"/>
+      <c r="I20" s="602"/>
       <c r="K20" s="19" t="s">
         <v>439</v>
       </c>
@@ -7651,7 +7626,7 @@
         <v>416</v>
       </c>
       <c r="P20" s="61" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="R20" s="24">
         <f>R18-SUM(X16:X21)+R26</f>
@@ -7671,7 +7646,7 @@
       <c r="X20" s="494"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="576"/>
+      <c r="I21" s="602"/>
       <c r="M21" s="221" t="s">
         <v>421</v>
       </c>
@@ -7701,9 +7676,9 @@
       <c r="G22" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I22" s="576"/>
+      <c r="I22" s="602"/>
       <c r="P22" s="99" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7716,7 +7691,7 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="576"/>
+      <c r="I23" s="602"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>5</v>
@@ -7733,7 +7708,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="576"/>
+      <c r="I24" s="602"/>
       <c r="U24" s="35"/>
       <c r="V24" s="541">
         <v>1</v>
@@ -7761,7 +7736,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="576"/>
+      <c r="I25" s="602"/>
       <c r="J25" s="421" t="s">
         <v>274</v>
       </c>
@@ -7806,7 +7781,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="576"/>
+      <c r="I26" s="602"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7841,7 +7816,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="576"/>
+      <c r="I27" s="602"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7868,7 +7843,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="576"/>
+      <c r="I28" s="602"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7890,7 +7865,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="577"/>
+      <c r="I29" s="603"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7948,6 +7923,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AH11:AK11"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
     <mergeCell ref="AB1:AB11"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
@@ -7961,11 +7941,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="AH11:AK11"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8041,7 +8016,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="593" t="s">
+      <c r="I1" s="590" t="s">
         <v>377</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -8077,7 +8052,7 @@
       <c r="X1" s="454" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="639" t="s">
+      <c r="Y1" s="646" t="s">
         <v>549</v>
       </c>
       <c r="Z1" s="430">
@@ -8102,7 +8077,7 @@
         <v>516</v>
       </c>
       <c r="AM1" s="426"/>
-      <c r="AN1" s="624"/>
+      <c r="AN1" s="628"/>
       <c r="AO1" s="350" t="s">
         <v>486</v>
       </c>
@@ -8111,23 +8086,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="648">
+      <c r="A2" s="610">
         <f ca="1">TODAY()</f>
-        <v>45280</v>
-      </c>
-      <c r="B2" s="650" t="s">
+        <v>45281</v>
+      </c>
+      <c r="B2" s="612" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="595" t="s">
+      <c r="C2" s="592" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="652" t="s">
+      <c r="D2" s="614" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="597" t="s">
+      <c r="E2" s="658" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="605" t="s">
+      <c r="F2" s="633" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="417" t="s">
@@ -8136,31 +8111,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="594"/>
+      <c r="I2" s="591"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="599" t="s">
+      <c r="K2" s="660" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="600"/>
-      <c r="M2" s="605" t="s">
+      <c r="L2" s="661"/>
+      <c r="M2" s="633" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="631" t="s">
+      <c r="O2" s="637" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="595" t="s">
+      <c r="Q2" s="592" t="s">
         <v>144</v>
       </c>
-      <c r="R2" s="557"/>
-      <c r="S2" s="618" t="s">
+      <c r="R2" s="561"/>
+      <c r="S2" s="650" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -8170,7 +8145,7 @@
       <c r="X2" s="455" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="640"/>
+      <c r="Y2" s="647"/>
       <c r="Z2" s="431">
         <v>1</v>
       </c>
@@ -8193,15 +8168,15 @@
         <v>480</v>
       </c>
       <c r="AM2" s="452"/>
-      <c r="AN2" s="625"/>
+      <c r="AN2" s="629"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="649"/>
-      <c r="B3" s="651"/>
-      <c r="C3" s="596"/>
-      <c r="D3" s="653"/>
-      <c r="E3" s="598"/>
-      <c r="F3" s="606"/>
+      <c r="A3" s="611"/>
+      <c r="B3" s="613"/>
+      <c r="C3" s="593"/>
+      <c r="D3" s="615"/>
+      <c r="E3" s="659"/>
+      <c r="F3" s="634"/>
       <c r="G3" s="418" t="s">
         <v>28</v>
       </c>
@@ -8220,17 +8195,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="606"/>
+      <c r="M3" s="634"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="632"/>
+      <c r="O3" s="638"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="596"/>
-      <c r="R3" s="559"/>
-      <c r="S3" s="620"/>
+      <c r="Q3" s="593"/>
+      <c r="R3" s="563"/>
+      <c r="S3" s="651"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -8238,7 +8213,7 @@
       <c r="X3" s="455" t="s">
         <v>158</v>
       </c>
-      <c r="Y3" s="640"/>
+      <c r="Y3" s="647"/>
       <c r="Z3" s="432">
         <v>1</v>
       </c>
@@ -8247,7 +8222,7 @@
       <c r="AC3" s="100" t="s">
         <v>497</v>
       </c>
-      <c r="AD3" s="615" t="s">
+      <c r="AD3" s="649" t="s">
         <v>472</v>
       </c>
       <c r="AE3" s="262"/>
@@ -8259,16 +8234,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="452"/>
-      <c r="AN3" s="625"/>
+      <c r="AN3" s="629"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="664" t="s">
+      <c r="B4" s="626" t="s">
         <v>381</v>
       </c>
-      <c r="C4" s="595" t="s">
+      <c r="C4" s="592" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -8277,7 +8252,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="606"/>
+      <c r="F4" s="634"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -8294,11 +8269,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="606"/>
+      <c r="M4" s="634"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="632"/>
+      <c r="O4" s="638"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -8320,12 +8295,12 @@
       <c r="X4" s="455" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="640"/>
+      <c r="Y4" s="647"/>
       <c r="Z4" s="433"/>
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="615"/>
+      <c r="AD4" s="649"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -8335,37 +8310,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="452"/>
-      <c r="AN4" s="625"/>
+      <c r="AN4" s="629"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="593" t="s">
+      <c r="A5" s="590" t="s">
         <v>434</v>
       </c>
-      <c r="B5" s="665"/>
-      <c r="C5" s="596"/>
+      <c r="B5" s="627"/>
+      <c r="C5" s="593"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="606"/>
-      <c r="G5" s="656" t="s">
+      <c r="F5" s="634"/>
+      <c r="G5" s="618" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="656"/>
-      <c r="I5" s="656"/>
-      <c r="J5" s="656"/>
-      <c r="K5" s="656"/>
-      <c r="L5" s="657"/>
-      <c r="M5" s="606"/>
+      <c r="H5" s="618"/>
+      <c r="I5" s="618"/>
+      <c r="J5" s="618"/>
+      <c r="K5" s="618"/>
+      <c r="L5" s="619"/>
+      <c r="M5" s="634"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="632"/>
+      <c r="O5" s="638"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8373,7 +8348,7 @@
       <c r="X5" s="455" t="s">
         <v>160</v>
       </c>
-      <c r="Y5" s="640"/>
+      <c r="Y5" s="647"/>
       <c r="Z5" s="433">
         <v>1</v>
       </c>
@@ -8396,24 +8371,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="452"/>
-      <c r="AN5" s="625"/>
+      <c r="AN5" s="629"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="594"/>
-      <c r="B6" s="662" t="s">
+      <c r="A6" s="591"/>
+      <c r="B6" s="624" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="591"/>
-      <c r="D6" s="592"/>
-      <c r="F6" s="606"/>
-      <c r="G6" s="658"/>
-      <c r="H6" s="658"/>
-      <c r="I6" s="658"/>
-      <c r="J6" s="658"/>
-      <c r="K6" s="658"/>
-      <c r="L6" s="659"/>
-      <c r="M6" s="606"/>
-      <c r="O6" s="632"/>
+      <c r="C6" s="588"/>
+      <c r="D6" s="589"/>
+      <c r="F6" s="634"/>
+      <c r="G6" s="620"/>
+      <c r="H6" s="620"/>
+      <c r="I6" s="620"/>
+      <c r="J6" s="620"/>
+      <c r="K6" s="620"/>
+      <c r="L6" s="621"/>
+      <c r="M6" s="634"/>
+      <c r="O6" s="638"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8423,7 +8398,7 @@
       <c r="X6" s="455" t="s">
         <v>161</v>
       </c>
-      <c r="Y6" s="640"/>
+      <c r="Y6" s="647"/>
       <c r="Z6" s="431">
         <v>1</v>
       </c>
@@ -8437,16 +8412,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="614"/>
+      <c r="AI6" s="643"/>
       <c r="AJ6" s="465" t="s">
         <v>475</v>
       </c>
-      <c r="AK6" s="614" t="s">
+      <c r="AK6" s="643" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="452"/>
-      <c r="AN6" s="625"/>
+      <c r="AN6" s="629"/>
       <c r="AO6" s="350" t="s">
         <v>487</v>
       </c>
@@ -8455,7 +8430,7 @@
       <c r="A7" s="237" t="s">
         <v>594</v>
       </c>
-      <c r="B7" s="663"/>
+      <c r="B7" s="625"/>
       <c r="C7" s="207" t="s">
         <v>382</v>
       </c>
@@ -8465,7 +8440,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="606"/>
+      <c r="F7" s="634"/>
       <c r="G7" s="419">
         <v>0</v>
       </c>
@@ -8478,14 +8453,14 @@
       <c r="J7" s="30">
         <v>0</v>
       </c>
-      <c r="K7" s="557">
+      <c r="K7" s="561">
         <v>0</v>
       </c>
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="606"/>
-      <c r="O7" s="632"/>
+      <c r="M7" s="634"/>
+      <c r="O7" s="638"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8499,7 +8474,7 @@
       <c r="X7" s="455" t="s">
         <v>162</v>
       </c>
-      <c r="Y7" s="640"/>
+      <c r="Y7" s="647"/>
       <c r="Z7" s="431">
         <v>1</v>
       </c>
@@ -8509,18 +8484,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="615" t="s">
+      <c r="AG7" s="649" t="s">
         <v>471</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="614"/>
+      <c r="AI7" s="643"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="614"/>
+      <c r="AK7" s="643"/>
       <c r="AL7" s="80" t="s">
         <v>514</v>
       </c>
       <c r="AM7" s="452"/>
-      <c r="AN7" s="625"/>
+      <c r="AN7" s="629"/>
       <c r="AP7" s="76" t="s">
         <v>488</v>
       </c>
@@ -8537,27 +8512,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="606"/>
-      <c r="G8" s="657">
-        <v>0</v>
-      </c>
-      <c r="H8" s="654" t="s">
+      <c r="F8" s="634"/>
+      <c r="G8" s="619">
+        <v>0</v>
+      </c>
+      <c r="H8" s="616" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="557">
-        <v>0</v>
-      </c>
-      <c r="J8" s="654" t="s">
+      <c r="I8" s="561">
+        <v>0</v>
+      </c>
+      <c r="J8" s="616" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="660"/>
-      <c r="L8" s="616"/>
-      <c r="M8" s="629"/>
-      <c r="N8" s="621">
+      <c r="K8" s="622"/>
+      <c r="L8" s="652"/>
+      <c r="M8" s="635"/>
+      <c r="N8" s="655">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="632"/>
+      <c r="O8" s="638"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8567,7 +8542,7 @@
       <c r="X8" s="455" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="640"/>
+      <c r="Y8" s="647"/>
       <c r="Z8" s="433"/>
       <c r="AA8" s="313"/>
       <c r="AB8" s="214"/>
@@ -8575,14 +8550,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="615"/>
+      <c r="AG8" s="649"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="614"/>
+      <c r="AI8" s="643"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="452"/>
-      <c r="AN8" s="625"/>
+      <c r="AN8" s="629"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8597,17 +8572,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="606"/>
-      <c r="G9" s="659"/>
-      <c r="H9" s="655"/>
-      <c r="I9" s="559"/>
-      <c r="J9" s="655"/>
-      <c r="K9" s="661"/>
-      <c r="L9" s="617"/>
-      <c r="M9" s="630"/>
-      <c r="N9" s="622"/>
-      <c r="O9" s="633"/>
-      <c r="S9" s="618" t="s">
+      <c r="F9" s="634"/>
+      <c r="G9" s="621"/>
+      <c r="H9" s="617"/>
+      <c r="I9" s="563"/>
+      <c r="J9" s="617"/>
+      <c r="K9" s="623"/>
+      <c r="L9" s="653"/>
+      <c r="M9" s="636"/>
+      <c r="N9" s="656"/>
+      <c r="O9" s="639"/>
+      <c r="S9" s="650" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8619,7 +8594,7 @@
       <c r="X9" s="455" t="s">
         <v>164</v>
       </c>
-      <c r="Y9" s="640"/>
+      <c r="Y9" s="647"/>
       <c r="Z9" s="434"/>
       <c r="AA9" s="313"/>
       <c r="AB9" s="214"/>
@@ -8629,16 +8604,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="615"/>
+      <c r="AG9" s="649"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="614"/>
+      <c r="AI9" s="643"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="614" t="s">
+      <c r="AK9" s="643" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="452"/>
-      <c r="AN9" s="625"/>
+      <c r="AN9" s="629"/>
       <c r="AP9" s="2" t="s">
         <v>526</v>
       </c>
@@ -8655,20 +8630,20 @@
         <f>Boat!U8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="606"/>
+      <c r="F10" s="634"/>
       <c r="N10" s="442" t="s">
         <v>406</v>
       </c>
-      <c r="O10" s="608" t="s">
+      <c r="O10" s="667" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="634" t="s">
+      <c r="P10" s="640" t="s">
         <v>410</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="619"/>
+      <c r="S10" s="654"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8680,7 +8655,7 @@
       <c r="X10" s="455" t="s">
         <v>165</v>
       </c>
-      <c r="Y10" s="640"/>
+      <c r="Y10" s="647"/>
       <c r="Z10" s="433">
         <v>0</v>
       </c>
@@ -8698,16 +8673,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="615"/>
+      <c r="AG10" s="649"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="614"/>
+      <c r="AI10" s="643"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="614"/>
+      <c r="AK10" s="643"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="466" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="625"/>
+      <c r="AN10" s="629"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8716,7 +8691,7 @@
       <c r="A11" s="228" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="557" t="s">
+      <c r="B11" s="561" t="s">
         <v>288</v>
       </c>
       <c r="C11" s="481" t="s">
@@ -8725,18 +8700,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="606"/>
+      <c r="F11" s="634"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="609"/>
-      <c r="P11" s="635"/>
+      <c r="O11" s="668"/>
+      <c r="P11" s="641"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="619"/>
+      <c r="S11" s="654"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8746,7 +8721,7 @@
       <c r="X11" s="455" t="s">
         <v>166</v>
       </c>
-      <c r="Y11" s="640"/>
+      <c r="Y11" s="647"/>
       <c r="Z11" s="433"/>
       <c r="AA11" s="313">
         <v>1</v>
@@ -8760,14 +8735,14 @@
       <c r="AF11" s="262" t="s">
         <v>493</v>
       </c>
-      <c r="AG11" s="615"/>
+      <c r="AG11" s="649"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="452"/>
-      <c r="AN11" s="625"/>
+      <c r="AN11" s="629"/>
       <c r="AP11" s="76" t="s">
         <v>501</v>
       </c>
@@ -8776,7 +8751,7 @@
       <c r="A12" s="232" t="s">
         <v>392</v>
       </c>
-      <c r="B12" s="559"/>
+      <c r="B12" s="563"/>
       <c r="C12" s="482" t="s">
         <v>393</v>
       </c>
@@ -8786,25 +8761,25 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="606"/>
+      <c r="F12" s="634"/>
       <c r="G12" s="349" t="s">
         <v>410</v>
       </c>
-      <c r="H12" s="562" t="s">
+      <c r="H12" s="566" t="s">
         <v>446</v>
       </c>
-      <c r="I12" s="564"/>
-      <c r="J12" s="564"/>
-      <c r="K12" s="613"/>
+      <c r="I12" s="568"/>
+      <c r="J12" s="568"/>
+      <c r="K12" s="672"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="609"/>
-      <c r="P12" s="635"/>
+      <c r="O12" s="668"/>
+      <c r="P12" s="641"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="620"/>
+      <c r="S12" s="651"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8814,7 +8789,7 @@
       <c r="X12" s="455" t="s">
         <v>167</v>
       </c>
-      <c r="Y12" s="640"/>
+      <c r="Y12" s="647"/>
       <c r="Z12" s="431">
         <v>1</v>
       </c>
@@ -8825,16 +8800,16 @@
       <c r="AC12" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD12" s="623" t="s">
+      <c r="AD12" s="657" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="465" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="615" t="s">
+      <c r="AF12" s="649" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="615"/>
+      <c r="AG12" s="649"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8844,10 +8819,10 @@
       <c r="AJ12" s="262"/>
       <c r="AK12" s="262"/>
       <c r="AL12" s="262"/>
-      <c r="AM12" s="637" t="s">
+      <c r="AM12" s="644" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="625"/>
+      <c r="AN12" s="629"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8859,17 +8834,17 @@
       <c r="E13" s="472">
         <v>-3</v>
       </c>
-      <c r="F13" s="606"/>
-      <c r="G13" s="564" t="s">
+      <c r="F13" s="634"/>
+      <c r="G13" s="568" t="s">
         <v>447</v>
       </c>
-      <c r="H13" s="564"/>
-      <c r="I13" s="564"/>
-      <c r="J13" s="613"/>
+      <c r="H13" s="568"/>
+      <c r="I13" s="568"/>
+      <c r="J13" s="672"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="609"/>
-      <c r="P13" s="636"/>
+      <c r="O13" s="668"/>
+      <c r="P13" s="642"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8879,7 +8854,7 @@
       <c r="X13" s="455" t="s">
         <v>168</v>
       </c>
-      <c r="Y13" s="640"/>
+      <c r="Y13" s="647"/>
       <c r="Z13" s="431">
         <v>1</v>
       </c>
@@ -8890,8 +8865,8 @@
         <v>518</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="623"/>
-      <c r="AF13" s="615"/>
+      <c r="AD13" s="657"/>
+      <c r="AF13" s="649"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8902,8 +8877,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
-      <c r="AM13" s="637"/>
-      <c r="AN13" s="625"/>
+      <c r="AM13" s="644"/>
+      <c r="AN13" s="629"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="474"/>
@@ -8911,18 +8886,18 @@
       <c r="C14" s="483"/>
       <c r="D14" s="476"/>
       <c r="E14" s="477"/>
-      <c r="F14" s="606"/>
-      <c r="G14" s="564" t="s">
+      <c r="F14" s="634"/>
+      <c r="G14" s="568" t="s">
         <v>446</v>
       </c>
-      <c r="H14" s="564"/>
-      <c r="I14" s="564"/>
-      <c r="J14" s="613"/>
+      <c r="H14" s="568"/>
+      <c r="I14" s="568"/>
+      <c r="J14" s="672"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="609"/>
+      <c r="O14" s="668"/>
       <c r="Q14" s="61" t="s">
         <v>553</v>
       </c>
@@ -8936,34 +8911,34 @@
       <c r="X14" s="455" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="640"/>
+      <c r="Y14" s="647"/>
       <c r="Z14" s="431">
         <v>1</v>
       </c>
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="623"/>
+      <c r="AD14" s="657"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="615"/>
+      <c r="AF14" s="649"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="262"/>
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
-      <c r="AM14" s="637"/>
-      <c r="AN14" s="625"/>
+      <c r="AM14" s="644"/>
+      <c r="AN14" s="629"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="473" t="s">
         <v>524</v>
       </c>
-      <c r="C15" s="557" t="s">
+      <c r="C15" s="561" t="s">
         <v>381</v>
       </c>
-      <c r="F15" s="606"/>
-      <c r="O15" s="609"/>
+      <c r="F15" s="634"/>
+      <c r="O15" s="668"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8976,7 +8951,7 @@
       <c r="X15" s="455" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="640"/>
+      <c r="Y15" s="647"/>
       <c r="Z15" s="433">
         <v>1</v>
       </c>
@@ -8985,8 +8960,8 @@
       <c r="AC15" s="76" t="s">
         <v>496</v>
       </c>
-      <c r="AD15" s="623"/>
-      <c r="AF15" s="615"/>
+      <c r="AD15" s="657"/>
+      <c r="AF15" s="649"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>465</v>
@@ -8999,8 +8974,8 @@
       </c>
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
-      <c r="AM15" s="637"/>
-      <c r="AN15" s="625"/>
+      <c r="AM15" s="644"/>
+      <c r="AN15" s="629"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -9015,20 +8990,20 @@
       <c r="B16" s="21" t="s">
         <v>416</v>
       </c>
-      <c r="C16" s="559"/>
+      <c r="C16" s="563"/>
       <c r="D16" s="61" t="s">
         <v>510</v>
       </c>
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="606"/>
+      <c r="F16" s="634"/>
       <c r="G16" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I16" s="495"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="609"/>
+      <c r="O16" s="668"/>
       <c r="R16" s="459" t="s">
         <v>185</v>
       </c>
@@ -9039,7 +9014,7 @@
       <c r="X16" s="455" t="s">
         <v>171</v>
       </c>
-      <c r="Y16" s="640"/>
+      <c r="Y16" s="647"/>
       <c r="Z16" s="431">
         <v>1</v>
       </c>
@@ -9060,18 +9035,18 @@
       <c r="AM16" s="452" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="625"/>
+      <c r="AN16" s="629"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="606"/>
+      <c r="F17" s="634"/>
       <c r="I17" s="496"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="609"/>
+      <c r="O17" s="668"/>
       <c r="Q17" s="21" t="s">
         <v>551</v>
       </c>
@@ -9091,7 +9066,7 @@
       <c r="X17" s="455" t="s">
         <v>172</v>
       </c>
-      <c r="Y17" s="640"/>
+      <c r="Y17" s="647"/>
       <c r="Z17" s="433"/>
       <c r="AA17" s="313"/>
       <c r="AB17" s="214"/>
@@ -9116,7 +9091,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="452"/>
-      <c r="AN17" s="625"/>
+      <c r="AN17" s="629"/>
       <c r="AO17" s="209" t="s">
         <v>515</v>
       </c>
@@ -9140,21 +9115,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="606"/>
+      <c r="F18" s="634"/>
       <c r="G18" s="349" t="s">
         <v>548</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="609"/>
+      <c r="O18" s="668"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="601" t="s">
+      <c r="R18" s="662" t="s">
         <v>556</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="645" t="s">
+      <c r="U18" s="607" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -9164,7 +9139,7 @@
       <c r="X18" s="455" t="s">
         <v>173</v>
       </c>
-      <c r="Y18" s="640"/>
+      <c r="Y18" s="647"/>
       <c r="Z18" s="433">
         <v>1</v>
       </c>
@@ -9175,38 +9150,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="614" t="s">
+      <c r="AF18" s="643" t="s">
         <v>492</v>
       </c>
       <c r="AG18" s="262"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="638" t="s">
+      <c r="AJ18" s="645" t="s">
         <v>322</v>
       </c>
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="452"/>
-      <c r="AN18" s="625"/>
+      <c r="AN18" s="629"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="606"/>
+      <c r="F19" s="634"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="609"/>
-      <c r="R19" s="602"/>
+      <c r="O19" s="668"/>
+      <c r="R19" s="663"/>
       <c r="S19" s="30" t="s">
         <v>554</v>
       </c>
-      <c r="U19" s="646"/>
+      <c r="U19" s="608"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="455" t="s">
         <v>174</v>
       </c>
-      <c r="Y19" s="640"/>
+      <c r="Y19" s="647"/>
       <c r="Z19" s="431">
         <v>1</v>
       </c>
@@ -9215,17 +9190,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="614"/>
+      <c r="AF19" s="643"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="638"/>
+      <c r="AJ19" s="645"/>
       <c r="AK19" s="484" t="s">
         <v>256</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="452"/>
-      <c r="AN19" s="625"/>
+      <c r="AN19" s="629"/>
       <c r="AP19" s="76" t="s">
         <v>485</v>
       </c>
@@ -9246,24 +9221,24 @@
       <c r="E20" s="461">
         <v>-1</v>
       </c>
-      <c r="F20" s="606"/>
+      <c r="F20" s="634"/>
       <c r="G20" s="349" t="s">
         <v>508</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="609"/>
-      <c r="Q20" s="611" t="s">
+      <c r="O20" s="668"/>
+      <c r="Q20" s="670" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="428" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="647"/>
+      <c r="U20" s="609"/>
       <c r="W20" s="429"/>
       <c r="X20" s="456" t="s">
         <v>175</v>
       </c>
-      <c r="Y20" s="640"/>
+      <c r="Y20" s="647"/>
       <c r="Z20" s="435">
         <v>1</v>
       </c>
@@ -9288,7 +9263,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="625"/>
+      <c r="AN20" s="629"/>
       <c r="AO20" s="350" t="s">
         <v>477</v>
       </c>
@@ -9309,20 +9284,20 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="606"/>
+      <c r="F21" s="634"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="609"/>
-      <c r="Q21" s="612"/>
+      <c r="O21" s="668"/>
+      <c r="Q21" s="671"/>
       <c r="T21" s="446"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="642"/>
+      <c r="V21" s="604"/>
       <c r="W21" s="450" t="s">
         <v>176</v>
       </c>
       <c r="X21" s="453" t="s">
         <v>187</v>
       </c>
-      <c r="Y21" s="640"/>
+      <c r="Y21" s="647"/>
       <c r="Z21" s="469">
         <v>3</v>
       </c>
@@ -9353,15 +9328,15 @@
       <c r="AM21" s="452" t="s">
         <v>565</v>
       </c>
-      <c r="AN21" s="625"/>
+      <c r="AN21" s="629"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="606"/>
+      <c r="F22" s="634"/>
       <c r="G22" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="609"/>
+      <c r="O22" s="668"/>
       <c r="R22" s="458" t="s">
         <v>44</v>
       </c>
@@ -9369,14 +9344,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="643"/>
+      <c r="V22" s="605"/>
       <c r="W22" s="450" t="s">
         <v>176</v>
       </c>
       <c r="X22" s="453" t="s">
         <v>188</v>
       </c>
-      <c r="Y22" s="640"/>
+      <c r="Y22" s="647"/>
       <c r="Z22" s="439"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="439"/>
@@ -9387,7 +9362,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="614" t="s">
+      <c r="AJ22" s="643" t="s">
         <v>489</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9395,7 +9370,7 @@
         <v>495</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="625"/>
+      <c r="AN22" s="629"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9413,22 +9388,22 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="606"/>
+      <c r="F23" s="634"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="609"/>
-      <c r="Q23" s="611" t="s">
+      <c r="O23" s="668"/>
+      <c r="Q23" s="670" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="444" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="643"/>
+      <c r="V23" s="605"/>
       <c r="W23" s="148"/>
       <c r="X23" s="453" t="s">
         <v>189</v>
       </c>
-      <c r="Y23" s="640"/>
+      <c r="Y23" s="647"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="439"/>
@@ -9439,13 +9414,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="614"/>
+      <c r="AJ23" s="643"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>525</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="625"/>
+      <c r="AN23" s="629"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="464" t="s">
@@ -9463,23 +9438,23 @@
       <c r="E24" s="460">
         <v>1</v>
       </c>
-      <c r="F24" s="606"/>
+      <c r="F24" s="634"/>
       <c r="G24" s="61" t="s">
         <v>507</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="609"/>
-      <c r="Q24" s="612"/>
+      <c r="O24" s="668"/>
+      <c r="Q24" s="671"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="643"/>
+      <c r="V24" s="605"/>
       <c r="W24" s="148"/>
       <c r="X24" s="453" t="s">
         <v>186</v>
       </c>
-      <c r="Y24" s="640"/>
+      <c r="Y24" s="647"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="439"/>
@@ -9498,12 +9473,12 @@
         <v>480</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="625"/>
+      <c r="AN24" s="629"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="606"/>
+      <c r="F25" s="634"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="609"/>
+      <c r="O25" s="668"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9516,12 +9491,12 @@
       <c r="U25" s="424" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="644"/>
+      <c r="V25" s="606"/>
       <c r="W25" s="148"/>
       <c r="X25" s="453" t="s">
         <v>190</v>
       </c>
-      <c r="Y25" s="640"/>
+      <c r="Y25" s="647"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="439"/>
@@ -9538,7 +9513,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="625"/>
+      <c r="AN25" s="629"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9556,17 +9531,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="606"/>
+      <c r="F26" s="634"/>
       <c r="G26" s="349" t="s">
         <v>504</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="609"/>
-      <c r="P26" s="627" t="s">
+      <c r="O26" s="668"/>
+      <c r="P26" s="631" t="s">
         <v>546</v>
       </c>
-      <c r="Q26" s="628"/>
-      <c r="R26" s="603" t="s">
+      <c r="Q26" s="632"/>
+      <c r="R26" s="664" t="s">
         <v>555</v>
       </c>
       <c r="T26" s="182"/>
@@ -9578,7 +9553,7 @@
       <c r="X26" s="453" t="s">
         <v>182</v>
       </c>
-      <c r="Y26" s="640"/>
+      <c r="Y26" s="647"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="439"/>
@@ -9605,7 +9580,7 @@
       <c r="AM26" s="466" t="s">
         <v>473</v>
       </c>
-      <c r="AN26" s="625"/>
+      <c r="AN26" s="629"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9617,13 +9592,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="607"/>
+      <c r="F27" s="666"/>
       <c r="G27" s="61" t="s">
         <v>564</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="610"/>
-      <c r="R27" s="604"/>
+      <c r="O27" s="669"/>
+      <c r="R27" s="665"/>
       <c r="S27" s="445" t="s">
         <v>54</v>
       </c>
@@ -9636,7 +9611,7 @@
       <c r="X27" s="453" t="s">
         <v>550</v>
       </c>
-      <c r="Y27" s="641"/>
+      <c r="Y27" s="648"/>
       <c r="Z27" s="163"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="440"/>
@@ -9653,10 +9628,48 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="626"/>
+      <c r="AN27" s="630"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9673,44 +9686,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9720,7 +9695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView topLeftCell="N3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AL18" sqref="AL18"/>
     </sheetView>
   </sheetViews>
@@ -9811,15 +9786,15 @@
       </c>
       <c r="R1" s="151">
         <f ca="1">TODAY()</f>
-        <v>45280</v>
+        <v>45281</v>
       </c>
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="669" t="s">
+      <c r="V1" s="680" t="s">
         <v>458</v>
       </c>
-      <c r="W1" s="670"/>
+      <c r="W1" s="681"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9835,21 +9810,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="671" t="s">
+      <c r="AC1" s="682" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="672"/>
-      <c r="AE1" s="673"/>
-      <c r="AF1" s="674" t="s">
+      <c r="AD1" s="683"/>
+      <c r="AE1" s="684"/>
+      <c r="AF1" s="685" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="675"/>
-      <c r="AH1" s="676"/>
-      <c r="AI1" s="666" t="s">
+      <c r="AG1" s="686"/>
+      <c r="AH1" s="687"/>
+      <c r="AI1" s="677" t="s">
         <v>461</v>
       </c>
-      <c r="AJ1" s="667"/>
-      <c r="AK1" s="668"/>
+      <c r="AJ1" s="678"/>
+      <c r="AK1" s="679"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9866,19 +9841,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="677">
+      <c r="L2" s="688">
         <f>SUM(L5:L30)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="679">
+      <c r="M2" s="690">
         <f>SUM(M4:M29)</f>
         <v>10</v>
       </c>
-      <c r="N2" s="681">
+      <c r="N2" s="692">
         <f>SUM(N4:N29)</f>
         <v>10</v>
       </c>
-      <c r="O2" s="621">
+      <c r="O2" s="655">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -9897,7 +9872,7 @@
       <c r="T2" s="510" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="683" t="s">
+      <c r="U2" s="694" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="511" t="s">
@@ -9966,10 +9941,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="678"/>
-      <c r="M3" s="680"/>
-      <c r="N3" s="682"/>
-      <c r="O3" s="622"/>
+      <c r="L3" s="689"/>
+      <c r="M3" s="691"/>
+      <c r="N3" s="693"/>
+      <c r="O3" s="656"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9985,7 +9960,7 @@
         <f>SUM(T4:T29)</f>
         <v>37</v>
       </c>
-      <c r="U3" s="684"/>
+      <c r="U3" s="695"/>
       <c r="V3" s="514">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>7</v>
@@ -10084,7 +10059,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="686" t="s">
+      <c r="O4" s="674" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -10163,7 +10138,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="687"/>
+      <c r="O5" s="675"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -10250,7 +10225,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="687"/>
+      <c r="O6" s="675"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -10344,7 +10319,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="687"/>
+      <c r="O7" s="675"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10452,7 +10427,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="687"/>
+      <c r="O8" s="675"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10536,7 +10511,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="687"/>
+      <c r="O9" s="675"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10630,7 +10605,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="687"/>
+      <c r="O10" s="675"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10713,7 +10688,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="687"/>
+      <c r="O11" s="675"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10773,7 +10748,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="657" t="s">
+      <c r="A12" s="619" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10782,7 +10757,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="611" t="s">
+      <c r="E12" s="670" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10803,7 +10778,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="687"/>
+      <c r="O12" s="675"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10875,14 +10850,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="659"/>
+      <c r="A13" s="621"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="612"/>
+      <c r="E13" s="671"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10905,7 +10880,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="687"/>
+      <c r="O13" s="675"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10981,7 +10956,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O14" s="687"/>
+      <c r="O14" s="675"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -11076,7 +11051,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="687"/>
+      <c r="O15" s="675"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -11163,7 +11138,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="687"/>
+      <c r="O16" s="675"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -11261,7 +11236,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O17" s="687"/>
+      <c r="O17" s="675"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -11356,7 +11331,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="687"/>
+      <c r="O18" s="675"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11439,7 +11414,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="687"/>
+      <c r="O19" s="675"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11537,11 +11512,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O20" s="688"/>
-      <c r="P20" s="562" t="s">
+      <c r="O20" s="676"/>
+      <c r="P20" s="566" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="613"/>
+      <c r="Q20" s="672"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11777,7 +11752,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="664" t="s">
+      <c r="E23" s="626" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11873,7 +11848,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="665"/>
+      <c r="E24" s="627"/>
       <c r="F24" s="176"/>
       <c r="H24" s="42">
         <v>-1</v>
@@ -11891,10 +11866,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P24" s="562" t="s">
+      <c r="P24" s="566" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="613"/>
+      <c r="Q24" s="672"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -12490,10 +12465,10 @@
       <c r="H32" s="42">
         <v>-1</v>
       </c>
-      <c r="I32" s="660" t="s">
+      <c r="I32" s="622" t="s">
         <v>609</v>
       </c>
-      <c r="J32" s="685"/>
+      <c r="J32" s="673"/>
       <c r="K32" s="406"/>
       <c r="L32" s="545">
         <v>0</v>
@@ -12977,13 +12952,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12993,6 +12961,13 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13027,15 +13002,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="562" t="s">
+      <c r="B1" s="566" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="613"/>
+      <c r="C1" s="672"/>
       <c r="D1" s="209"/>
-      <c r="J1" s="562" t="s">
+      <c r="J1" s="566" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="613"/>
+      <c r="K1" s="672"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -13073,13 +13048,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="201"/>
-      <c r="M2" s="689"/>
+      <c r="M2" s="696"/>
       <c r="N2" s="154">
         <v>2</v>
       </c>
       <c r="O2" s="155"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="692" t="s">
+      <c r="Q2" s="699" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="19">
@@ -13102,13 +13077,13 @@
       <c r="K3" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="M3" s="690"/>
+      <c r="M3" s="697"/>
       <c r="N3" s="17">
         <v>1</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="693"/>
+      <c r="Q3" s="700"/>
       <c r="R3" s="224"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13127,13 +13102,13 @@
       <c r="K4" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="M4" s="690"/>
+      <c r="M4" s="697"/>
       <c r="N4" s="17"/>
       <c r="O4" s="15">
         <v>1</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="693"/>
+      <c r="Q4" s="700"/>
       <c r="R4" s="224"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13153,13 +13128,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="201"/>
-      <c r="M5" s="690"/>
+      <c r="M5" s="697"/>
       <c r="N5" s="17">
         <v>1</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="693"/>
+      <c r="Q5" s="700"/>
       <c r="R5" s="19">
         <v>-1</v>
       </c>
@@ -13180,13 +13155,13 @@
       <c r="K6" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="M6" s="690"/>
+      <c r="M6" s="697"/>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="693"/>
+      <c r="Q6" s="700"/>
       <c r="R6" s="224"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13206,13 +13181,13 @@
         <v>334</v>
       </c>
       <c r="L7" s="203"/>
-      <c r="M7" s="690"/>
+      <c r="M7" s="697"/>
       <c r="N7" s="17">
         <v>1</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="693"/>
+      <c r="Q7" s="700"/>
       <c r="R7" s="19">
         <v>-1</v>
       </c>
@@ -13233,13 +13208,13 @@
       <c r="K8" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="M8" s="690"/>
+      <c r="M8" s="697"/>
       <c r="N8" s="17">
         <v>1</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="693"/>
+      <c r="Q8" s="700"/>
       <c r="R8" s="224"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13259,13 +13234,13 @@
         <v>336</v>
       </c>
       <c r="L9" s="185"/>
-      <c r="M9" s="691"/>
+      <c r="M9" s="698"/>
       <c r="N9" s="163"/>
       <c r="O9" s="18"/>
       <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="694"/>
+      <c r="Q9" s="701"/>
       <c r="R9" s="225"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -13421,12 +13396,12 @@
       <c r="P1" s="38"/>
       <c r="S1" s="58">
         <f ca="1">TODAY()</f>
-        <v>45280</v>
-      </c>
-      <c r="V1" s="562" t="s">
+        <v>45281</v>
+      </c>
+      <c r="V1" s="566" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="613"/>
+      <c r="W1" s="672"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13445,7 +13420,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="702" t="s">
+      <c r="AD1" s="716" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13462,10 +13437,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="701" t="s">
+      <c r="F2" s="747" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="729" t="s">
+      <c r="G2" s="704" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13493,10 +13468,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="669" t="s">
+      <c r="V2" s="680" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="670"/>
+      <c r="W2" s="681"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13515,7 +13490,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="703"/>
+      <c r="AD2" s="717"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13534,8 +13509,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="661"/>
-      <c r="G3" s="730"/>
+      <c r="F3" s="623"/>
+      <c r="G3" s="705"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13546,13 +13521,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="739" t="s">
+      <c r="O3" s="714" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="721" t="s">
+      <c r="P3" s="735" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="722"/>
+      <c r="Q3" s="736"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13562,15 +13537,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="703"/>
+      <c r="AD3" s="717"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="730"/>
+      <c r="G4" s="705"/>
       <c r="H4" s="6"/>
-      <c r="L4" s="692" t="s">
+      <c r="L4" s="699" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="740"/>
+      <c r="O4" s="715"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13580,12 +13555,12 @@
       <c r="X4" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="562" t="s">
+      <c r="Y4" s="566" t="s">
         <v>195</v>
       </c>
-      <c r="Z4" s="564"/>
-      <c r="AA4" s="613"/>
-      <c r="AD4" s="703"/>
+      <c r="Z4" s="568"/>
+      <c r="AA4" s="672"/>
+      <c r="AD4" s="717"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13600,21 +13575,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="730"/>
+      <c r="G5" s="705"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="708" t="s">
+      <c r="K5" s="722" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="723"/>
+      <c r="L5" s="737"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="740"/>
+      <c r="O5" s="715"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13630,11 +13605,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="711" t="s">
+      <c r="Y5" s="725" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="712"/>
-      <c r="AD5" s="703"/>
+      <c r="Z5" s="726"/>
+      <c r="AD5" s="717"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13644,16 +13619,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="730"/>
+      <c r="G6" s="705"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="709"/>
-      <c r="L6" s="723"/>
-      <c r="O6" s="740"/>
+      <c r="K6" s="723"/>
+      <c r="L6" s="737"/>
+      <c r="O6" s="715"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13663,23 +13638,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="703"/>
+      <c r="AD6" s="717"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="730"/>
+      <c r="G7" s="705"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="709"/>
-      <c r="L7" s="723"/>
+      <c r="K7" s="723"/>
+      <c r="L7" s="737"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="740"/>
+      <c r="O7" s="715"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="703"/>
+      <c r="AD7" s="717"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13692,7 +13667,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="730"/>
+      <c r="G8" s="705"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13702,41 +13677,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="709"/>
-      <c r="L8" s="723"/>
-      <c r="O8" s="740"/>
+      <c r="K8" s="723"/>
+      <c r="L8" s="737"/>
+      <c r="O8" s="715"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="705" t="s">
+      <c r="S8" s="719" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="706"/>
-      <c r="U8" s="706"/>
-      <c r="V8" s="706"/>
-      <c r="W8" s="706"/>
-      <c r="X8" s="706"/>
-      <c r="Y8" s="706"/>
-      <c r="Z8" s="706"/>
-      <c r="AA8" s="706"/>
-      <c r="AB8" s="706"/>
-      <c r="AC8" s="707"/>
-      <c r="AD8" s="703"/>
+      <c r="T8" s="720"/>
+      <c r="U8" s="720"/>
+      <c r="V8" s="720"/>
+      <c r="W8" s="720"/>
+      <c r="X8" s="720"/>
+      <c r="Y8" s="720"/>
+      <c r="Z8" s="720"/>
+      <c r="AA8" s="720"/>
+      <c r="AB8" s="720"/>
+      <c r="AC8" s="721"/>
+      <c r="AD8" s="717"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="695"/>
-      <c r="G9" s="730"/>
+      <c r="C9" s="741"/>
+      <c r="G9" s="705"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="709"/>
-      <c r="L9" s="733" t="s">
+      <c r="K9" s="723"/>
+      <c r="L9" s="708" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="734"/>
-      <c r="N9" s="735"/>
-      <c r="O9" s="740"/>
+      <c r="M9" s="709"/>
+      <c r="N9" s="710"/>
+      <c r="O9" s="715"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="703"/>
+      <c r="AD9" s="717"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="696"/>
+      <c r="C10" s="742"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13744,7 +13719,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="730"/>
+      <c r="G10" s="705"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13752,33 +13727,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="709"/>
-      <c r="M10" s="698" t="s">
+      <c r="K10" s="723"/>
+      <c r="M10" s="744" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="699"/>
-      <c r="O10" s="699"/>
-      <c r="P10" s="699"/>
-      <c r="Q10" s="699"/>
-      <c r="R10" s="699"/>
-      <c r="S10" s="699"/>
-      <c r="T10" s="699"/>
-      <c r="U10" s="699"/>
-      <c r="V10" s="699"/>
-      <c r="W10" s="699"/>
-      <c r="X10" s="699"/>
-      <c r="Y10" s="699"/>
-      <c r="Z10" s="699"/>
-      <c r="AA10" s="699"/>
-      <c r="AB10" s="699"/>
-      <c r="AC10" s="700"/>
-      <c r="AD10" s="703"/>
+      <c r="N10" s="745"/>
+      <c r="O10" s="745"/>
+      <c r="P10" s="745"/>
+      <c r="Q10" s="745"/>
+      <c r="R10" s="745"/>
+      <c r="S10" s="745"/>
+      <c r="T10" s="745"/>
+      <c r="U10" s="745"/>
+      <c r="V10" s="745"/>
+      <c r="W10" s="745"/>
+      <c r="X10" s="745"/>
+      <c r="Y10" s="745"/>
+      <c r="Z10" s="745"/>
+      <c r="AA10" s="745"/>
+      <c r="AB10" s="745"/>
+      <c r="AC10" s="746"/>
+      <c r="AD10" s="717"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="697"/>
-      <c r="G11" s="730"/>
+      <c r="C11" s="743"/>
+      <c r="G11" s="705"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="709"/>
+      <c r="K11" s="723"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13786,17 +13761,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="719" t="s">
+      <c r="Z11" s="733" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="720"/>
+      <c r="AA11" s="734"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="703"/>
+      <c r="AD11" s="717"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13809,7 +13784,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="730"/>
+      <c r="G12" s="705"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13817,8 +13792,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="709"/>
-      <c r="L12" s="724" t="s">
+      <c r="K12" s="723"/>
+      <c r="L12" s="738" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13833,7 +13808,7 @@
       <c r="Q12" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="557" t="s">
+      <c r="S12" s="561" t="s">
         <v>107</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -13849,26 +13824,26 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="713" t="s">
+      <c r="AA12" s="727" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="714"/>
+      <c r="AB12" s="728"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="703"/>
+      <c r="AD12" s="717"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="695"/>
-      <c r="G13" s="730"/>
-      <c r="K13" s="709"/>
-      <c r="L13" s="725"/>
+      <c r="C13" s="741"/>
+      <c r="G13" s="705"/>
+      <c r="K13" s="723"/>
+      <c r="L13" s="739"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="732" t="s">
+      <c r="Q13" s="707" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="628"/>
-      <c r="S13" s="558"/>
+      <c r="R13" s="632"/>
+      <c r="S13" s="562"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
         <v>132</v>
@@ -13876,17 +13851,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="715"/>
-      <c r="AB13" s="716"/>
-      <c r="AD13" s="703"/>
+      <c r="AA13" s="729"/>
+      <c r="AB13" s="730"/>
+      <c r="AD13" s="717"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="697"/>
+      <c r="C14" s="743"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="730"/>
+      <c r="G14" s="705"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13894,8 +13869,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="709"/>
-      <c r="L14" s="725"/>
+      <c r="K14" s="723"/>
+      <c r="L14" s="739"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13905,7 +13880,7 @@
       <c r="R14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="558"/>
+      <c r="S14" s="562"/>
       <c r="T14" s="77" t="s">
         <v>130</v>
       </c>
@@ -13916,9 +13891,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="715"/>
-      <c r="AB14" s="716"/>
-      <c r="AD14" s="703"/>
+      <c r="AA14" s="729"/>
+      <c r="AB14" s="730"/>
+      <c r="AD14" s="717"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13933,20 +13908,20 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="730"/>
+      <c r="G15" s="705"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="709"/>
-      <c r="L15" s="726"/>
-      <c r="Q15" s="732" t="s">
+      <c r="K15" s="723"/>
+      <c r="L15" s="740"/>
+      <c r="Q15" s="707" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="628"/>
-      <c r="S15" s="558"/>
+      <c r="R15" s="632"/>
+      <c r="S15" s="562"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
         <v>44</v>
@@ -13954,14 +13929,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="715"/>
-      <c r="AB15" s="716"/>
-      <c r="AD15" s="703"/>
+      <c r="AA15" s="729"/>
+      <c r="AB15" s="730"/>
+      <c r="AD15" s="717"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="730"/>
-      <c r="K16" s="709"/>
+      <c r="G16" s="705"/>
+      <c r="K16" s="723"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13969,7 +13944,7 @@
       <c r="R16" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="558"/>
+      <c r="S16" s="562"/>
       <c r="T16" s="76" t="s">
         <v>129</v>
       </c>
@@ -13980,34 +13955,34 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="715"/>
-      <c r="AB16" s="716"/>
-      <c r="AD16" s="703"/>
+      <c r="AA16" s="729"/>
+      <c r="AB16" s="730"/>
+      <c r="AD16" s="717"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="727" t="s">
+      <c r="F17" s="702" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="730"/>
+      <c r="G17" s="705"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="709"/>
-      <c r="S17" s="558"/>
+      <c r="K17" s="723"/>
+      <c r="S17" s="562"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="715"/>
-      <c r="AB17" s="716"/>
-      <c r="AD17" s="703"/>
+      <c r="AA17" s="729"/>
+      <c r="AB17" s="730"/>
+      <c r="AD17" s="717"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14017,61 +13992,58 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="728"/>
-      <c r="G18" s="730"/>
+      <c r="F18" s="703"/>
+      <c r="G18" s="705"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="709"/>
+      <c r="K18" s="723"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="S18" s="558"/>
+      <c r="S18" s="562"/>
       <c r="U18" s="76" t="s">
         <v>133</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="717"/>
-      <c r="AB18" s="718"/>
-      <c r="AD18" s="703"/>
+      <c r="AA18" s="731"/>
+      <c r="AB18" s="732"/>
+      <c r="AD18" s="717"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="731"/>
-      <c r="K19" s="710"/>
+      <c r="G19" s="706"/>
+      <c r="K19" s="724"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="736" t="s">
+      <c r="R19" s="711" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="737"/>
-      <c r="T19" s="738"/>
+      <c r="S19" s="712"/>
+      <c r="T19" s="713"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="704"/>
+      <c r="AD19" s="718"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14083,11 +14055,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>